<commit_message>
Adicionadas novas tabelas ao dicionário
Adicionadas as tabelas: Imóvel e Avaliação
Corrigidos os índices de todas as tabelas, feitos com base nas consultas
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario.xlsx
+++ b/dicionario_dados/dicionario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruni\Downloads\Trabalho de banco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\TRABANCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BB0918-A981-444D-85FC-4AA5ECC01614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C50B55-FE2E-4D98-AFE4-7E37165ED46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="72">
   <si>
     <t>Tabela</t>
   </si>
@@ -125,9 +125,6 @@
     <t>decimal</t>
   </si>
   <si>
-    <t>Código de identificador da apólice</t>
-  </si>
-  <si>
     <t>Código de identificador do cliente vinculado</t>
   </si>
   <si>
@@ -155,10 +152,106 @@
     <t>id_apolice, id_imovel</t>
   </si>
   <si>
-    <t>Idx_id_cliente</t>
-  </si>
-  <si>
-    <t>id_apolice, id_cliente</t>
+    <t>Tabela responsável por armazenar os dados do imóvel assegurado</t>
+  </si>
+  <si>
+    <t>id_proprietario</t>
+  </si>
+  <si>
+    <t>endereco</t>
+  </si>
+  <si>
+    <t>tipo_imovel</t>
+  </si>
+  <si>
+    <t>area_imovel</t>
+  </si>
+  <si>
+    <t>ano_construcao</t>
+  </si>
+  <si>
+    <t>valor_imovel</t>
+  </si>
+  <si>
+    <t>id_inquilino</t>
+  </si>
+  <si>
+    <t>Código identificador da apólice</t>
+  </si>
+  <si>
+    <t>Código identificador do imóvel</t>
+  </si>
+  <si>
+    <t>Código de identificador do inquilino vinculado</t>
+  </si>
+  <si>
+    <t>Código de identificador do proprietário vinculado</t>
+  </si>
+  <si>
+    <t>Imovel</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>Endereço onde o imóvel se encontra</t>
+  </si>
+  <si>
+    <t>1 a 4</t>
+  </si>
+  <si>
+    <t>Ano de construção do Imóvel</t>
+  </si>
+  <si>
+    <t>Área ocupada pelo imóvel</t>
+  </si>
+  <si>
+    <t>Valor de compra e venda do imóvel</t>
+  </si>
+  <si>
+    <t>Tipologia da construção do imóvel (Casa, Apt.)</t>
+  </si>
+  <si>
+    <t>id_imovel, tipo_imovel</t>
+  </si>
+  <si>
+    <t>Idx_id_imovel_tipo_imovel</t>
+  </si>
+  <si>
+    <t>Avaliacao</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados de avaliação de imóveis assegurados</t>
+  </si>
+  <si>
+    <t>id_avaliacao</t>
+  </si>
+  <si>
+    <t>dt_avaliacao</t>
+  </si>
+  <si>
+    <t>valor_avaliado</t>
+  </si>
+  <si>
+    <t>Idx_id_avaliacao</t>
+  </si>
+  <si>
+    <t>Idx_id_avaliacao_id_imovel</t>
+  </si>
+  <si>
+    <t>id_avaliacao, id_imovel</t>
+  </si>
+  <si>
+    <t>Valor avaliado de cobertura do imóvel</t>
+  </si>
+  <si>
+    <t>data da avaliação</t>
+  </si>
+  <si>
+    <t>Código de identificador do imóvel</t>
+  </si>
+  <si>
+    <t>Código identificador da avaliacao</t>
   </si>
 </sst>
 </file>
@@ -202,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -226,16 +319,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -244,51 +346,74 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,47 +745,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,144 +806,144 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -828,82 +953,630 @@
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="11" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="14"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="6"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="49">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="B1:H1"/>
@@ -917,12 +1590,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adicionada a tabela Pagamento no dicionário
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario.xlsx
+++ b/dicionario_dados/dicionario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3d59f93496549/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5794EB-D1AE-4441-9565-6F226739BCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{AD5794EB-D1AE-4441-9565-6F226739BCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{968C0427-526D-4631-9B12-476A4FF92382}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-23148" yWindow="-96" windowWidth="23256" windowHeight="12456" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="111">
   <si>
     <t>Tabela</t>
   </si>
@@ -348,13 +348,34 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Pagamento</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados de pagamentos</t>
+  </si>
+  <si>
+    <t>id_pagamento</t>
+  </si>
+  <si>
+    <t>Código identificador do pagamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador da apólice </t>
+  </si>
+  <si>
+    <t>Data do pagamento</t>
+  </si>
+  <si>
+    <t>Valor de pagamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +387,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -475,19 +504,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -499,23 +531,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,47 +890,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -909,10 +951,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
@@ -931,10 +973,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
@@ -953,10 +995,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
@@ -973,10 +1015,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
@@ -993,10 +1035,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1013,22 +1055,22 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1038,17 +1080,17 @@
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1056,17 +1098,17 @@
       <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3" t="s">
         <v>11</v>
@@ -1074,57 +1116,57 @@
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1145,10 +1187,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1167,10 +1209,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1189,10 +1231,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1211,10 +1253,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1231,10 +1273,10 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1251,10 +1293,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1271,10 +1313,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1291,10 +1333,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1323,10 +1365,10 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1336,17 +1378,17 @@
       <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1354,17 +1396,17 @@
       <c r="E30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3" t="s">
         <v>11</v>
@@ -1372,57 +1414,57 @@
       <c r="E31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="16"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
@@ -1443,10 +1485,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="17"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1465,10 +1507,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="2" t="s">
         <v>8</v>
       </c>
@@ -1487,10 +1529,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2" t="s">
         <v>27</v>
       </c>
@@ -1507,10 +1549,10 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="17"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="2" t="s">
         <v>28</v>
       </c>
@@ -1539,10 +1581,10 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="16"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
         <v>12</v>
       </c>
@@ -1552,17 +1594,17 @@
       <c r="E42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="15"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
@@ -1570,17 +1612,17 @@
       <c r="E43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="15"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="15"/>
+      <c r="B44" s="7"/>
       <c r="C44" s="4"/>
       <c r="D44" s="3" t="s">
         <v>11</v>
@@ -1588,57 +1630,57 @@
       <c r="E44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="16"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1659,10 +1701,10 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="17"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="2" t="s">
         <v>8</v>
       </c>
@@ -1681,10 +1723,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B51" s="17"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="2" t="s">
         <v>8</v>
       </c>
@@ -1703,10 +1745,10 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="11"/>
+      <c r="B52" s="16"/>
       <c r="C52" s="2" t="s">
         <v>27</v>
       </c>
@@ -1723,10 +1765,10 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="17"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="2" t="s">
         <v>28</v>
       </c>
@@ -1743,10 +1785,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="9"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1755,10 +1797,10 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="16"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
         <v>12</v>
       </c>
@@ -1768,17 +1810,17 @@
       <c r="E55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="15"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="4" t="s">
         <v>11</v>
       </c>
@@ -1786,57 +1828,57 @@
       <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="16"/>
+      <c r="B61" s="12"/>
       <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
@@ -1857,10 +1899,10 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="17"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="2" t="s">
         <v>8</v>
       </c>
@@ -1879,10 +1921,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="17"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="2" t="s">
         <v>8</v>
       </c>
@@ -1913,10 +1955,10 @@
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="16"/>
+      <c r="B65" s="12"/>
       <c r="C65" s="1" t="s">
         <v>12</v>
       </c>
@@ -1926,67 +1968,67 @@
       <c r="E65" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="16" t="s">
+      <c r="F65" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="4"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="16"/>
+      <c r="B71" s="12"/>
       <c r="C71" s="1" t="s">
         <v>4</v>
       </c>
@@ -2007,10 +2049,10 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="17"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="2" t="s">
         <v>8</v>
       </c>
@@ -2029,10 +2071,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="17"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="2" t="s">
         <v>47</v>
       </c>
@@ -2049,10 +2091,10 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="17"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="2" t="s">
         <v>28</v>
       </c>
@@ -2069,10 +2111,10 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B75" s="9"/>
+      <c r="B75" s="20"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -2081,10 +2123,10 @@
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B76" s="9"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="1" t="s">
         <v>12</v>
       </c>
@@ -2094,67 +2136,67 @@
       <c r="E76" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="8"/>
-      <c r="H76" s="9"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="20"/>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="15"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="4"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+      <c r="A82" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="16"/>
+      <c r="B82" s="12"/>
       <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
@@ -2175,10 +2217,10 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="17"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="2" t="s">
         <v>8</v>
       </c>
@@ -2197,10 +2239,10 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="17"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="2" t="s">
         <v>47</v>
       </c>
@@ -2217,10 +2259,10 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="20"/>
+      <c r="B85" s="10"/>
       <c r="C85" s="2" t="s">
         <v>27</v>
       </c>
@@ -2237,10 +2279,10 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="11"/>
+      <c r="B86" s="16"/>
       <c r="C86" s="2" t="s">
         <v>47</v>
       </c>
@@ -2257,10 +2299,10 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="20"/>
+      <c r="B87" s="10"/>
       <c r="C87" s="2" t="s">
         <v>47</v>
       </c>
@@ -2277,10 +2319,10 @@
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="20"/>
+      <c r="B88" s="10"/>
       <c r="C88" s="2" t="s">
         <v>47</v>
       </c>
@@ -2297,10 +2339,10 @@
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B89" s="9"/>
+      <c r="B89" s="20"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -2309,10 +2351,10 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B90" s="9"/>
+      <c r="B90" s="20"/>
       <c r="C90" s="1" t="s">
         <v>12</v>
       </c>
@@ -2322,90 +2364,227 @@
       <c r="E90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F90" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G90" s="8"/>
-      <c r="H90" s="9"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="20"/>
     </row>
     <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="B91" s="15"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
       <c r="C91" s="4"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="15"/>
-      <c r="H91" s="15"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" s="12"/>
+      <c r="C96" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G96" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" s="22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="J97" s="21"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H98" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D100" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" s="20"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="20"/>
+      <c r="C102" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102" s="19"/>
+      <c r="H102" s="20"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="98">
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="A81:H81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="F56:H56"/>
+  <mergeCells count="111">
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
@@ -2422,22 +2601,89 @@
     <mergeCell ref="B69:H69"/>
     <mergeCell ref="A70:H70"/>
     <mergeCell ref="A65:B65"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="A81:H81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A91:B91"/>
     <mergeCell ref="F90:H90"/>
     <mergeCell ref="A90:B90"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A86:B86"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A54:B54"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
rename idx_id_imovel to idx_id_apolice_id_imovel
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario.xlsx
+++ b/dicionario_dados/dicionario.xlsx
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -384,8 +384,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,8 +428,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,8 +443,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -429,47 +460,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -507,7 +500,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,7 +515,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,13 +534,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -556,7 +556,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,7 +598,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,31 +652,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,102 +724,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -724,19 +736,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,6 +802,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -817,41 +832,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,151 +884,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5740740740741" defaultRowHeight="14.4"/>

</xml_diff>